<commit_message>
editing the path to extract from zip file
</commit_message>
<xml_diff>
--- a/performance_results.xlsx
+++ b/performance_results.xlsx
@@ -475,22 +475,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>12.91661310195923</v>
+        <v>110.0884997844696</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9422546083979826</v>
+        <v>0.540052929905726</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9422546083979826</v>
+        <v>0.540052929905726</v>
       </c>
       <c r="E2" t="n">
-        <v>13.46586728096008</v>
+        <v>95.08698892593384</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9038213407482136</v>
+        <v>0.6252550167914027</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9038213407482136</v>
+        <v>0.6252550167914027</v>
       </c>
     </row>
     <row r="3">
@@ -498,22 +498,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>8.803105592727661</v>
+        <v>43.52274942398071</v>
       </c>
       <c r="C3" t="n">
-        <v>1.382550520610501</v>
+        <v>1.366035410087631</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6912752603052507</v>
+        <v>0.6830177050438153</v>
       </c>
       <c r="E3" t="n">
-        <v>8.990721940994263</v>
+        <v>41.95485782623291</v>
       </c>
       <c r="F3" t="n">
-        <v>1.353699769617045</v>
+        <v>1.417085408888084</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6768498848085224</v>
+        <v>0.7085427044440419</v>
       </c>
     </row>
     <row r="4">
@@ -521,22 +521,22 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>7.840163946151733</v>
+        <v>25.15734624862671</v>
       </c>
       <c r="C4" t="n">
-        <v>1.552357616984365</v>
+        <v>2.363270603741606</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3880894042460913</v>
+        <v>0.5908176509354016</v>
       </c>
       <c r="E4" t="n">
-        <v>7.905767202377319</v>
+        <v>25.50388050079346</v>
       </c>
       <c r="F4" t="n">
-        <v>1.539475917853364</v>
+        <v>2.331159638850998</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3848689794633409</v>
+        <v>0.5827899097127495</v>
       </c>
     </row>
     <row r="5">
@@ -544,22 +544,22 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>7.638689279556274</v>
+        <v>21.81533575057983</v>
       </c>
       <c r="C5" t="n">
-        <v>1.593301910157266</v>
+        <v>2.725312942109931</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1991627387696583</v>
+        <v>0.3406641177637414</v>
       </c>
       <c r="E5" t="n">
-        <v>8.722803831100464</v>
+        <v>24.43703198432922</v>
       </c>
       <c r="F5" t="n">
-        <v>1.395278221988788</v>
+        <v>2.432931171660069</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1744097777485985</v>
+        <v>0.3041163964575087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated code with multiprocessing and multithreading
</commit_message>
<xml_diff>
--- a/performance_results.xlsx
+++ b/performance_results.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Performance_Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Multiprocessing_Logs" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Threading_Logs" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -475,22 +477,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>12.91661310195923</v>
+        <v>126.1362450122833</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9422546083979826</v>
+        <v>1.004751468006303</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9422546083979826</v>
+        <v>1.004751468006303</v>
       </c>
       <c r="E2" t="n">
-        <v>13.46586728096008</v>
+        <v>142.5983219146729</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9038213407482136</v>
+        <v>0.888759247957558</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9038213407482136</v>
+        <v>0.888759247957558</v>
       </c>
     </row>
     <row r="3">
@@ -498,22 +500,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>8.803105592727661</v>
+        <v>95.04795742034912</v>
       </c>
       <c r="C3" t="n">
-        <v>1.382550520610501</v>
+        <v>1.333385595909304</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6912752603052507</v>
+        <v>0.6666927979546522</v>
       </c>
       <c r="E3" t="n">
-        <v>8.990721940994263</v>
+        <v>78.20663857460022</v>
       </c>
       <c r="F3" t="n">
-        <v>1.353699769617045</v>
+        <v>1.620521987068951</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6768498848085224</v>
+        <v>0.8102609935344754</v>
       </c>
     </row>
     <row r="4">
@@ -521,22 +523,22 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>7.840163946151733</v>
+        <v>55.80835247039795</v>
       </c>
       <c r="C4" t="n">
-        <v>1.552357616984365</v>
+        <v>2.270906983181736</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3880894042460913</v>
+        <v>0.567726745795434</v>
       </c>
       <c r="E4" t="n">
-        <v>7.905767202377319</v>
+        <v>51.40283536911011</v>
       </c>
       <c r="F4" t="n">
-        <v>1.539475917853364</v>
+        <v>2.465536705024925</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3848689794633409</v>
+        <v>0.6163841762562312</v>
       </c>
     </row>
     <row r="5">
@@ -544,22 +546,984 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>7.638689279556274</v>
+        <v>72.31622862815857</v>
       </c>
       <c r="C5" t="n">
-        <v>1.593301910157266</v>
+        <v>1.752519175143295</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1991627387696583</v>
+        <v>0.2190648968929119</v>
       </c>
       <c r="E5" t="n">
-        <v>8.722803831100464</v>
+        <v>42.97739434242249</v>
       </c>
       <c r="F5" t="n">
-        <v>1.395278221988788</v>
+        <v>2.948889277351912</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1744097777485985</v>
+        <v>0.3686111596689891</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>chunk_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>core_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pid</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>start_time</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>end_time</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>total_process</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>9532</v>
+      </c>
+      <c r="D2" t="n">
+        <v>16764</v>
+      </c>
+      <c r="E2" t="n">
+        <v>124.5641024112701</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1767041910.949548</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1767042035.51365</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>29080</v>
+      </c>
+      <c r="D3" t="n">
+        <v>12640</v>
+      </c>
+      <c r="E3" t="n">
+        <v>91.01139426231384</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1767042038.553832</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1767042129.565227</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>13240</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10056</v>
+      </c>
+      <c r="E4" t="n">
+        <v>91.96164631843567</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1767042038.593357</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1767042130.555003</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>6604</v>
+      </c>
+      <c r="D5" t="n">
+        <v>8448</v>
+      </c>
+      <c r="E5" t="n">
+        <v>50.84522175788879</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1767042134.529646</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1767042185.374867</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>26216</v>
+      </c>
+      <c r="D6" t="n">
+        <v>11516</v>
+      </c>
+      <c r="E6" t="n">
+        <v>50.83322739601135</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1767042134.558581</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1767042185.391808</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>22992</v>
+      </c>
+      <c r="D7" t="n">
+        <v>22328</v>
+      </c>
+      <c r="E7" t="n">
+        <v>51.78951406478882</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1767042134.56843</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1767042186.357944</v>
+      </c>
+      <c r="H7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>17276</v>
+      </c>
+      <c r="D8" t="n">
+        <v>760</v>
+      </c>
+      <c r="E8" t="n">
+        <v>51.31769466400146</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1767042134.636961</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1767042185.954656</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>29468</v>
+      </c>
+      <c r="D9" t="n">
+        <v>14040</v>
+      </c>
+      <c r="E9" t="n">
+        <v>64.25694155693054</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1767042192.998388</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1767042257.255329</v>
+      </c>
+      <c r="H9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>28996</v>
+      </c>
+      <c r="D10" t="n">
+        <v>29440</v>
+      </c>
+      <c r="E10" t="n">
+        <v>65.47787809371948</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1767042193.137343</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1767042258.615222</v>
+      </c>
+      <c r="H10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>11748</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1228</v>
+      </c>
+      <c r="E11" t="n">
+        <v>64.80469799041748</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1767042193.284628</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1767042258.089326</v>
+      </c>
+      <c r="H11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>24676</v>
+      </c>
+      <c r="D12" t="n">
+        <v>18376</v>
+      </c>
+      <c r="E12" t="n">
+        <v>63.49760723114014</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1767042193.298851</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1767042256.796458</v>
+      </c>
+      <c r="H12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>15208</v>
+      </c>
+      <c r="D13" t="n">
+        <v>18144</v>
+      </c>
+      <c r="E13" t="n">
+        <v>64.61180806159973</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1767042193.345564</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1767042257.957372</v>
+      </c>
+      <c r="H13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>5</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>27776</v>
+      </c>
+      <c r="D14" t="n">
+        <v>26752</v>
+      </c>
+      <c r="E14" t="n">
+        <v>65.15985989570618</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1767042193.508028</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1767042258.667888</v>
+      </c>
+      <c r="H14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>6</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>23152</v>
+      </c>
+      <c r="D15" t="n">
+        <v>19848</v>
+      </c>
+      <c r="E15" t="n">
+        <v>64.50136661529541</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1767042193.61279</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1767042258.114157</v>
+      </c>
+      <c r="H15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>7</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>23488</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5436</v>
+      </c>
+      <c r="E16" t="n">
+        <v>64.69863629341125</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1767042193.661934</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1767042258.36057</v>
+      </c>
+      <c r="H16" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>chunk_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>core_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pid</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>start_time</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>end_time</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>total_workers</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1120</v>
+      </c>
+      <c r="E2" t="n">
+        <v>142.5936994552612</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1767042258.739631</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1767042401.33333</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D3" t="n">
+        <v>15700</v>
+      </c>
+      <c r="E3" t="n">
+        <v>77.95184779167175</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1767042401.336055</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1767042479.287902</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D4" t="n">
+        <v>17084</v>
+      </c>
+      <c r="E4" t="n">
+        <v>78.20398187637329</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1767042401.336653</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1767042479.540635</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D5" t="n">
+        <v>11740</v>
+      </c>
+      <c r="E5" t="n">
+        <v>50.54696178436279</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1767042479.543628</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1767042530.09059</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D6" t="n">
+        <v>25260</v>
+      </c>
+      <c r="E6" t="n">
+        <v>51.01939821243286</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1767042479.544106</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1767042530.563505</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D7" t="n">
+        <v>22080</v>
+      </c>
+      <c r="E7" t="n">
+        <v>51.3218846321106</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1767042479.545362</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1767042530.867246</v>
+      </c>
+      <c r="H7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D8" t="n">
+        <v>29516</v>
+      </c>
+      <c r="E8" t="n">
+        <v>51.39917850494385</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1767042479.544692</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1767042530.94387</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D9" t="n">
+        <v>12348</v>
+      </c>
+      <c r="E9" t="n">
+        <v>41.92096567153931</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1767042530.949184</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1767042572.870149</v>
+      </c>
+      <c r="H9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D10" t="n">
+        <v>28020</v>
+      </c>
+      <c r="E10" t="n">
+        <v>42.46502065658569</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1767042530.950034</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1767042573.415054</v>
+      </c>
+      <c r="H10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D11" t="n">
+        <v>19468</v>
+      </c>
+      <c r="E11" t="n">
+        <v>42.53934550285339</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1767042530.947589</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1767042573.486934</v>
+      </c>
+      <c r="H11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D12" t="n">
+        <v>26600</v>
+      </c>
+      <c r="E12" t="n">
+        <v>42.54424047470093</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1767042530.952155</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1767042573.496395</v>
+      </c>
+      <c r="H12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5052</v>
+      </c>
+      <c r="E13" t="n">
+        <v>42.77667927742004</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1767042530.94703</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1767042573.723709</v>
+      </c>
+      <c r="H13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D14" t="n">
+        <v>192</v>
+      </c>
+      <c r="E14" t="n">
+        <v>42.84362840652466</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1767042530.953012</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1767042573.79664</v>
+      </c>
+      <c r="H14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D15" t="n">
+        <v>18896</v>
+      </c>
+      <c r="E15" t="n">
+        <v>42.93406867980957</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1767042530.948409</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1767042573.882478</v>
+      </c>
+      <c r="H15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>5</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>28476</v>
+      </c>
+      <c r="D16" t="n">
+        <v>25528</v>
+      </c>
+      <c r="E16" t="n">
+        <v>42.96966910362244</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1767042530.95131</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1767042573.920979</v>
+      </c>
+      <c r="H16" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add multithreading and modify output
</commit_message>
<xml_diff>
--- a/performance_results.xlsx
+++ b/performance_results.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Performance" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Logs_Multiprocessing" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Logs_Threading" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -475,22 +477,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>12.91661310195923</v>
+        <v>198.9427213668823</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9422546083979826</v>
+        <v>0.755771751534011</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9422546083979826</v>
+        <v>0.755771751534011</v>
       </c>
       <c r="E2" t="n">
-        <v>13.46586728096008</v>
+        <v>196.7172567844391</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9038213407482136</v>
+        <v>0.7643218060281781</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9038213407482136</v>
+        <v>0.7643218060281781</v>
       </c>
     </row>
     <row r="3">
@@ -498,22 +500,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>8.803105592727661</v>
+        <v>103.2628507614136</v>
       </c>
       <c r="C3" t="n">
-        <v>1.382550520610501</v>
+        <v>1.45604433611642</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6912752603052507</v>
+        <v>0.7280221680582099</v>
       </c>
       <c r="E3" t="n">
-        <v>8.990721940994263</v>
+        <v>108.9537482261658</v>
       </c>
       <c r="F3" t="n">
-        <v>1.353699769617045</v>
+        <v>1.379991890414678</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6768498848085224</v>
+        <v>0.689995945207339</v>
       </c>
     </row>
     <row r="4">
@@ -521,22 +523,22 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>7.840163946151733</v>
+        <v>50.31356406211853</v>
       </c>
       <c r="C4" t="n">
-        <v>1.552357616984365</v>
+        <v>2.988364902886993</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3880894042460913</v>
+        <v>0.7470912257217484</v>
       </c>
       <c r="E4" t="n">
-        <v>7.905767202377319</v>
+        <v>53.06745147705078</v>
       </c>
       <c r="F4" t="n">
-        <v>1.539475917853364</v>
+        <v>2.833286408099192</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3848689794633409</v>
+        <v>0.708321602024798</v>
       </c>
     </row>
     <row r="5">
@@ -544,22 +546,684 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>7.638689279556274</v>
+        <v>39.34957480430603</v>
       </c>
       <c r="C5" t="n">
-        <v>1.593301910157266</v>
+        <v>3.821014324300601</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1991627387696583</v>
+        <v>0.4776267905375751</v>
       </c>
       <c r="E5" t="n">
-        <v>8.722803831100464</v>
+        <v>35.88936758041382</v>
       </c>
       <c r="F5" t="n">
-        <v>1.395278221988788</v>
+        <v>4.189410377474745</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1744097777485985</v>
+        <v>0.5236762971843432</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>chunk_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>core_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pid</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>41184</v>
+      </c>
+      <c r="D2" t="n">
+        <v>73004</v>
+      </c>
+      <c r="E2" t="n">
+        <v>196.0459661483765</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>71460</v>
+      </c>
+      <c r="D3" t="n">
+        <v>100376</v>
+      </c>
+      <c r="E3" t="n">
+        <v>99.7650830745697</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>40264</v>
+      </c>
+      <c r="D4" t="n">
+        <v>58720</v>
+      </c>
+      <c r="E4" t="n">
+        <v>97.84637141227722</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>54884</v>
+      </c>
+      <c r="D5" t="n">
+        <v>54564</v>
+      </c>
+      <c r="E5" t="n">
+        <v>46.1568443775177</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>64312</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4016</v>
+      </c>
+      <c r="E6" t="n">
+        <v>45.68017840385437</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>11464</v>
+      </c>
+      <c r="D7" t="n">
+        <v>48264</v>
+      </c>
+      <c r="E7" t="n">
+        <v>46.6286633014679</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>19040</v>
+      </c>
+      <c r="D8" t="n">
+        <v>81472</v>
+      </c>
+      <c r="E8" t="n">
+        <v>46.19452142715454</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>27840</v>
+      </c>
+      <c r="D9" t="n">
+        <v>15736</v>
+      </c>
+      <c r="E9" t="n">
+        <v>35.39994144439697</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>15328</v>
+      </c>
+      <c r="D10" t="n">
+        <v>18604</v>
+      </c>
+      <c r="E10" t="n">
+        <v>35.0500385761261</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>83180</v>
+      </c>
+      <c r="D11" t="n">
+        <v>32128</v>
+      </c>
+      <c r="E11" t="n">
+        <v>35.96310496330261</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>25972</v>
+      </c>
+      <c r="D12" t="n">
+        <v>89800</v>
+      </c>
+      <c r="E12" t="n">
+        <v>34.95152902603149</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>61704</v>
+      </c>
+      <c r="D13" t="n">
+        <v>21996</v>
+      </c>
+      <c r="E13" t="n">
+        <v>35.0556948184967</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>47664</v>
+      </c>
+      <c r="D14" t="n">
+        <v>34328</v>
+      </c>
+      <c r="E14" t="n">
+        <v>35.97525382041931</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>7</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>41704</v>
+      </c>
+      <c r="D15" t="n">
+        <v>63368</v>
+      </c>
+      <c r="E15" t="n">
+        <v>35.09989786148071</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>8</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>39448</v>
+      </c>
+      <c r="D16" t="n">
+        <v>73804</v>
+      </c>
+      <c r="E16" t="n">
+        <v>35.62797856330872</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>chunk_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>core_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pid</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D2" t="n">
+        <v>100540</v>
+      </c>
+      <c r="E2" t="n">
+        <v>196.7172567844391</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D3" t="n">
+        <v>33648</v>
+      </c>
+      <c r="E3" t="n">
+        <v>108.3031725883484</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D4" t="n">
+        <v>41724</v>
+      </c>
+      <c r="E4" t="n">
+        <v>108.9537482261658</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D5" t="n">
+        <v>52384</v>
+      </c>
+      <c r="E5" t="n">
+        <v>52.93813991546631</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D6" t="n">
+        <v>77132</v>
+      </c>
+      <c r="E6" t="n">
+        <v>52.98183059692383</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D7" t="n">
+        <v>26044</v>
+      </c>
+      <c r="E7" t="n">
+        <v>53.05931997299194</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D8" t="n">
+        <v>11680</v>
+      </c>
+      <c r="E8" t="n">
+        <v>52.97369909286499</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D9" t="n">
+        <v>57392</v>
+      </c>
+      <c r="E9" t="n">
+        <v>34.91174602508545</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D10" t="n">
+        <v>67792</v>
+      </c>
+      <c r="E10" t="n">
+        <v>35.55812048912048</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D11" t="n">
+        <v>68776</v>
+      </c>
+      <c r="E11" t="n">
+        <v>35.88936758041382</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D12" t="n">
+        <v>36412</v>
+      </c>
+      <c r="E12" t="n">
+        <v>35.23008942604065</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D13" t="n">
+        <v>89400</v>
+      </c>
+      <c r="E13" t="n">
+        <v>35.67280435562134</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D14" t="n">
+        <v>93828</v>
+      </c>
+      <c r="E14" t="n">
+        <v>35.50208330154419</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>7</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D15" t="n">
+        <v>15828</v>
+      </c>
+      <c r="E15" t="n">
+        <v>35.0648627281189</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>8</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>76128</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3844</v>
+      </c>
+      <c r="E16" t="n">
+        <v>35.35245037078857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>